<commit_message>
Apply employment share per BU rather than boolean isEmployed in employment alignment
- This modification applies a new method fracEmployed() to compute simulated employment share in ActivityAlignmentV2.java
- employment targets in "policy parameters.xlsx" have been updated accordingly
</commit_message>
<xml_diff>
--- a/input/PL/policy parameters.xlsx
+++ b/input/PL/policy parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEUmerged/input/PL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBA0A1F-39C2-5041-B201-5BA9BC6FC05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBE2FD0-18E0-9341-A850-6D5B10C9221B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23520" yWindow="500" windowWidth="25560" windowHeight="25900" firstSheet="6" activeTab="6" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
+    <workbookView xWindow="20100" yWindow="500" windowWidth="28980" windowHeight="27600" firstSheet="5" activeTab="10" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="disability" sheetId="10" r:id="rId1"/>
@@ -711,7 +711,7 @@
         <v>2011</v>
       </c>
       <c r="B2">
-        <v>0.36003186935365528</v>
+        <v>0.38052187841351931</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -719,7 +719,7 @@
         <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.38692491437698423</v>
+        <v>0.39494946229994121</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -727,7 +727,7 @@
         <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.36132873647659114</v>
+        <v>0.3708155540743337</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -735,7 +735,7 @@
         <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.38088347179059528</v>
+        <v>0.39400614231074099</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -743,7 +743,7 @@
         <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.38498832940988709</v>
+        <v>0.39038070193201418</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -751,7 +751,7 @@
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.4058379925777626</v>
+        <v>0.4045626857325601</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -759,7 +759,7 @@
         <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.43108781433921883</v>
+        <v>0.43452589116520407</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -767,7 +767,7 @@
         <v>2018</v>
       </c>
       <c r="B9">
-        <v>0.40755919614401981</v>
+        <v>0.41769307045724119</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -775,7 +775,7 @@
         <v>2019</v>
       </c>
       <c r="B10">
-        <v>0.42056689824920096</v>
+        <v>0.42367705016359092</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -783,7 +783,7 @@
         <v>2020</v>
       </c>
       <c r="B11">
-        <v>0.45737911395870984</v>
+        <v>0.45367977278524363</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -791,7 +791,7 @@
         <v>2021</v>
       </c>
       <c r="B12">
-        <v>0.45357219704792257</v>
+        <v>0.44799750636445951</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -799,7 +799,7 @@
         <v>2022</v>
       </c>
       <c r="B13">
-        <v>0.4353627057118411</v>
+        <v>0.43338321233616106</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -807,7 +807,7 @@
         <v>2023</v>
       </c>
       <c r="B14">
-        <v>0.41823639194988294</v>
+        <v>0.43184882342437486</v>
       </c>
     </row>
   </sheetData>
@@ -819,7 +819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D3E0F8-B7AE-434D-A980-C4586EF714A7}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
@@ -841,7 +841,7 @@
         <v>2011</v>
       </c>
       <c r="B2">
-        <v>0.51128277630011854</v>
+        <v>0.51193623756613316</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -849,7 +849,7 @@
         <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.51393263199108286</v>
+        <v>0.51388796407993187</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -857,7 +857,7 @@
         <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.5076697666645027</v>
+        <v>0.50731054213776516</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -865,7 +865,7 @@
         <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.51067476163189951</v>
+        <v>0.51131531460632029</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -873,7 +873,7 @@
         <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.53577002132648832</v>
+        <v>0.53318545452592403</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -881,7 +881,7 @@
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.58570650522171619</v>
+        <v>0.58285048457054911</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -889,7 +889,7 @@
         <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.59110843342391406</v>
+        <v>0.59181134292156978</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -897,7 +897,7 @@
         <v>2018</v>
       </c>
       <c r="B9">
-        <v>0.56825257026071563</v>
+        <v>0.56828787809135639</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -905,7 +905,7 @@
         <v>2019</v>
       </c>
       <c r="B10">
-        <v>0.57190222490428488</v>
+        <v>0.57210350926861453</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -913,7 +913,7 @@
         <v>2020</v>
       </c>
       <c r="B11">
-        <v>0.56928754219274136</v>
+        <v>0.56859266378921847</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -921,7 +921,7 @@
         <v>2021</v>
       </c>
       <c r="B12">
-        <v>0.61268070477504499</v>
+        <v>0.61407456424300411</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -929,7 +929,7 @@
         <v>2022</v>
       </c>
       <c r="B13">
-        <v>0.59899189733983293</v>
+        <v>0.60188645030954646</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -937,7 +937,7 @@
         <v>2023</v>
       </c>
       <c r="B14">
-        <v>0.59106341164084708</v>
+        <v>0.59164974063354814</v>
       </c>
     </row>
   </sheetData>
@@ -971,7 +971,7 @@
         <v>2011</v>
       </c>
       <c r="B2">
-        <v>0.61680769920349121</v>
+        <v>0.30785190812656721</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -979,7 +979,7 @@
         <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.61431878805160522</v>
+        <v>0.30811218783286087</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -987,7 +987,7 @@
         <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.62226575613021851</v>
+        <v>0.31195865499437081</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -995,7 +995,7 @@
         <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.56901419162750244</v>
+        <v>0.28581726919907879</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1003,7 +1003,7 @@
         <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.55749976634979248</v>
+        <v>0.27963714773111775</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1011,7 +1011,7 @@
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.61379510164260864</v>
+        <v>0.30752858106411018</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1019,7 +1019,7 @@
         <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.60692942142486572</v>
+        <v>0.30346469681990601</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1027,7 +1027,7 @@
         <v>2018</v>
       </c>
       <c r="B9">
-        <v>0.62670052051544189</v>
+        <v>0.31364752176359245</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1035,7 +1035,7 @@
         <v>2019</v>
       </c>
       <c r="B10">
-        <v>0.70763528347015381</v>
+        <v>0.35381764642659308</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1043,7 +1043,7 @@
         <v>2020</v>
       </c>
       <c r="B11">
-        <v>0.69641482830047607</v>
+        <v>0.34820741422940238</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1051,7 +1051,7 @@
         <v>2021</v>
       </c>
       <c r="B12">
-        <v>0.72090119123458862</v>
+        <v>0.3607173104243539</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1059,7 +1059,7 @@
         <v>2022</v>
       </c>
       <c r="B13">
-        <v>0.72393757104873657</v>
+        <v>0.36274965739361886</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1067,7 +1067,7 @@
         <v>2023</v>
       </c>
       <c r="B14">
-        <v>0.73154628276824951</v>
+        <v>0.36845418733118185</v>
       </c>
     </row>
   </sheetData>
@@ -1101,7 +1101,7 @@
         <v>2011</v>
       </c>
       <c r="B2">
-        <v>0.83789324760437012</v>
+        <v>0.41894661081369583</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1109,7 +1109,7 @@
         <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.80550128221511841</v>
+        <v>0.40321361657827082</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1117,7 +1117,7 @@
         <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.7992321252822876</v>
+        <v>0.39961607117918457</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1125,7 +1125,7 @@
         <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.79625046253204346</v>
+        <v>0.39812522211769624</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1133,7 +1133,7 @@
         <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.81983458995819092</v>
+        <v>0.40991729842040864</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1141,7 +1141,7 @@
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.81091392040252686</v>
+        <v>0.40545695127308695</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1149,7 +1149,7 @@
         <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.82456725835800171</v>
+        <v>0.41228362735812552</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1157,7 +1157,7 @@
         <v>2018</v>
       </c>
       <c r="B9">
-        <v>0.85373425483703613</v>
+        <v>0.42686713226978734</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1165,7 +1165,7 @@
         <v>2019</v>
       </c>
       <c r="B10">
-        <v>0.84969794750213623</v>
+        <v>0.42517186848982991</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1173,7 +1173,7 @@
         <v>2020</v>
       </c>
       <c r="B11">
-        <v>0.82026958465576172</v>
+        <v>0.41013480515252171</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1181,7 +1181,7 @@
         <v>2021</v>
       </c>
       <c r="B12">
-        <v>0.86517715454101562</v>
+        <v>0.43258856779953725</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1189,7 +1189,7 @@
         <v>2022</v>
       </c>
       <c r="B13">
-        <v>0.88653171062469482</v>
+        <v>0.44326586886465918</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1197,7 +1197,7 @@
         <v>2023</v>
       </c>
       <c r="B14">
-        <v>0.92414480447769165</v>
+        <v>0.46207239052048033</v>
       </c>
     </row>
   </sheetData>
@@ -3584,7 +3584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C02B2D7-F4EC-4D40-840B-FB6BA99B9F2B}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
@@ -3603,7 +3603,7 @@
         <v>2011</v>
       </c>
       <c r="B2">
-        <v>0.44670278305339939</v>
+        <v>0.44580390908196338</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3611,7 +3611,7 @@
         <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.44336450393902516</v>
+        <v>0.44324938187318652</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -3619,7 +3619,7 @@
         <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.44440277662332139</v>
+        <v>0.44437298985301549</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -3627,7 +3627,7 @@
         <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.45769354631775144</v>
+        <v>0.45665144279125908</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -3635,7 +3635,7 @@
         <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.46857670454141603</v>
+        <v>0.47060122836212664</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3643,7 +3643,7 @@
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.46135340171417216</v>
+        <v>0.46283571902209464</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -3651,7 +3651,7 @@
         <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.48381900646628939</v>
+        <v>0.4829455027595948</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3659,7 +3659,7 @@
         <v>2018</v>
       </c>
       <c r="B9">
-        <v>0.4911795212142166</v>
+        <v>0.49083580436737168</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -3667,7 +3667,7 @@
         <v>2019</v>
       </c>
       <c r="B10">
-        <v>0.48726882873224336</v>
+        <v>0.48680351073667416</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -3675,7 +3675,7 @@
         <v>2020</v>
       </c>
       <c r="B11">
-        <v>0.49614597341437744</v>
+        <v>0.49651737484706926</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -3683,7 +3683,7 @@
         <v>2021</v>
       </c>
       <c r="B12">
-        <v>0.52459623426267399</v>
+        <v>0.52320974701450895</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -3691,7 +3691,7 @@
         <v>2022</v>
       </c>
       <c r="B13">
-        <v>0.53915577006649817</v>
+        <v>0.53678039526990218</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -3699,7 +3699,7 @@
         <v>2023</v>
       </c>
       <c r="B14">
-        <v>0.52156811285163618</v>
+        <v>0.52108578146447826</v>
       </c>
     </row>
   </sheetData>
@@ -3730,7 +3730,7 @@
         <v>2011</v>
       </c>
       <c r="B2">
-        <v>0.31394928614821893</v>
+        <v>0.30208181732795336</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3738,7 +3738,7 @@
         <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.30848042060514502</v>
+        <v>0.30061108532233771</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -3746,7 +3746,7 @@
         <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.30956841493744147</v>
+        <v>0.30276407721188736</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -3754,7 +3754,7 @@
         <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.31944256894108353</v>
+        <v>0.31145040929785739</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -3762,7 +3762,7 @@
         <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.31710955870099683</v>
+        <v>0.31244190895581908</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3770,7 +3770,7 @@
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.31537141978390892</v>
+        <v>0.31288817157553944</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -3778,7 +3778,7 @@
         <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.31503917525773195</v>
+        <v>0.30967743686400945</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3786,7 +3786,7 @@
         <v>2018</v>
       </c>
       <c r="B9">
-        <v>0.31132235685019893</v>
+        <v>0.3052372997493929</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -3794,7 +3794,7 @@
         <v>2019</v>
       </c>
       <c r="B10">
-        <v>0.3186277678079098</v>
+        <v>0.31519769527800484</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -3802,7 +3802,7 @@
         <v>2020</v>
       </c>
       <c r="B11">
-        <v>0.31556614940666167</v>
+        <v>0.31410432759222856</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -3810,7 +3810,7 @@
         <v>2021</v>
       </c>
       <c r="B12">
-        <v>0.32083228970536581</v>
+        <v>0.319650585035544</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -3818,7 +3818,7 @@
         <v>2022</v>
       </c>
       <c r="B13">
-        <v>0.34580404255112251</v>
+        <v>0.34466439690323852</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -3826,7 +3826,7 @@
         <v>2023</v>
       </c>
       <c r="B14">
-        <v>0.34735164074624669</v>
+        <v>0.34069381864858117</v>
       </c>
     </row>
   </sheetData>
@@ -3857,7 +3857,7 @@
         <v>2011</v>
       </c>
       <c r="B2">
-        <v>0.97541612386703491</v>
+        <v>0.82383029192035362</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3865,7 +3865,7 @@
         <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.97455012798309326</v>
+        <v>0.821731322462114</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -3873,7 +3873,7 @@
         <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.96620428562164307</v>
+        <v>0.81609950788251906</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -3881,7 +3881,7 @@
         <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.97489017248153687</v>
+        <v>0.83106676793864132</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -3889,7 +3889,7 @@
         <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.9752197265625</v>
+        <v>0.83335242550016386</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3897,7 +3897,7 @@
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.98048520088195801</v>
+        <v>0.83973543797809402</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -3905,7 +3905,7 @@
         <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.97633326053619385</v>
+        <v>0.84157973500650807</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3913,7 +3913,7 @@
         <v>2018</v>
       </c>
       <c r="B9">
-        <v>0.98472893238067627</v>
+        <v>0.84545298666168944</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -3921,7 +3921,7 @@
         <v>2019</v>
       </c>
       <c r="B10">
-        <v>0.98302763700485229</v>
+        <v>0.8534134938695962</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -3929,7 +3929,7 @@
         <v>2020</v>
       </c>
       <c r="B11">
-        <v>0.98899710178375244</v>
+        <v>0.86500591632281076</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -3937,7 +3937,7 @@
         <v>2021</v>
       </c>
       <c r="B12">
-        <v>0.99124062061309814</v>
+        <v>0.88091732038400394</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -3945,7 +3945,7 @@
         <v>2022</v>
       </c>
       <c r="B13">
-        <v>0.9915042519569397</v>
+        <v>0.87862197711765877</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -3953,7 +3953,7 @@
         <v>2023</v>
       </c>
       <c r="B14">
-        <v>0.99202412366867065</v>
+        <v>0.89231035103286582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>